<commit_message>
CIERRE 13 SEP 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/BALANCE  ZAVALETA   AGOSTO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/BALANCE  ZAVALETA   AGOSTO    2023.xlsx
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="906">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -3315,6 +3315,33 @@
   </si>
   <si>
     <t>NOMINA # 31 Y Vac. Rosa B</t>
+  </si>
+  <si>
+    <t>QUESOS-JAMON-CHORIZO</t>
+  </si>
+  <si>
+    <t>Lomos-Jamones-Quesos-Pollo-Salsas-Longaniza-Pastor-arabe- verduras</t>
+  </si>
+  <si>
+    <t>Jamon-Quesos-Pollo-Salchicha-Aros cebolla-Salchicha-Bimbo</t>
+  </si>
+  <si>
+    <t>Jamon-queso pco-quesos-pollo-salsas</t>
+  </si>
+  <si>
+    <t>PASTOR-QUESOS-POLLO-POSTRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLLO-QUESO   </t>
+  </si>
+  <si>
+    <t>PASTOR-JAMON-QUESOS-POLLO-CREMA-MANTEQUILLA</t>
+  </si>
+  <si>
+    <t>NOMINA # 32</t>
+  </si>
+  <si>
+    <t>Nomina # 32</t>
   </si>
 </sst>
 </file>
@@ -6016,6 +6043,39 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6090,39 +6150,6 @@
     </xf>
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10001,23 +10028,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -10027,24 +10054,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="543" t="s">
+      <c r="R3" s="554" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10059,14 +10086,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -10076,11 +10103,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="544"/>
+      <c r="R4" s="555"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -11915,11 +11942,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -11927,7 +11954,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -11948,10 +11975,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -12006,11 +12033,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -12435,26 +12462,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="562" t="s">
+      <c r="H77" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="563"/>
+      <c r="I77" s="574"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="564">
+      <c r="K77" s="575">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="565"/>
+      <c r="L77" s="576"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="556" t="s">
+      <c r="D78" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="556"/>
+      <c r="E78" s="567"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -12463,22 +12490,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="557" t="s">
+      <c r="D79" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="557"/>
+      <c r="E79" s="568"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="558" t="s">
+      <c r="I79" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="559"/>
-      <c r="K79" s="560">
+      <c r="J79" s="570"/>
+      <c r="K79" s="571">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="560"/>
+      <c r="L79" s="571"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -12519,11 +12546,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="561">
+      <c r="K81" s="572">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="560"/>
+      <c r="L81" s="571"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -12540,22 +12567,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="549" t="s">
+      <c r="D83" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="550"/>
+      <c r="E83" s="561"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="551" t="s">
+      <c r="I83" s="562" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="552"/>
-      <c r="K83" s="553">
+      <c r="J83" s="563"/>
+      <c r="K83" s="564">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="553"/>
+      <c r="L83" s="564"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -12702,12 +12729,6 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -12724,6 +12745,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15122,23 +15149,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -15148,21 +15175,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -15183,14 +15210,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -15200,7 +15227,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -17260,11 +17287,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -17272,7 +17299,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -17305,10 +17332,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -17393,11 +17420,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -17726,26 +17753,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="562" t="s">
+      <c r="H69" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="563"/>
+      <c r="I69" s="574"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="564">
+      <c r="K69" s="575">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="565"/>
+      <c r="L69" s="576"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="556" t="s">
+      <c r="D70" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="556"/>
+      <c r="E70" s="567"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -17754,23 +17781,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="557" t="s">
+      <c r="D71" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="557"/>
+      <c r="E71" s="568"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="558" t="s">
+      <c r="I71" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="559"/>
-      <c r="K71" s="560">
+      <c r="J71" s="570"/>
+      <c r="K71" s="571">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="560"/>
+      <c r="L71" s="571"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -17812,11 +17839,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="561">
+      <c r="K73" s="572">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="560"/>
+      <c r="L73" s="571"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -17833,22 +17860,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="549" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="550"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="551" t="s">
+      <c r="I75" s="562" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="552"/>
-      <c r="K75" s="553">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="553"/>
+      <c r="L75" s="564"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -17996,6 +18023,12 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -18012,12 +18045,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -20417,23 +20444,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -20443,21 +20470,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -20476,14 +20503,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -20493,7 +20520,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -22584,11 +22611,11 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>2422108.7600000002</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1603736</v>
       </c>
@@ -22596,7 +22623,7 @@
         <f>SUM(P5:P40)</f>
         <v>4927758.76</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>-0.23999999999068677</v>
       </c>
@@ -22623,10 +22650,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>440369</v>
@@ -22693,11 +22720,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>4025844.7600000002</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -22980,26 +23007,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="562" t="s">
+      <c r="H69" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="563"/>
+      <c r="I69" s="574"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="564">
+      <c r="K69" s="575">
         <f>I67+L67</f>
         <v>594414.23</v>
       </c>
-      <c r="L69" s="565"/>
+      <c r="L69" s="576"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="556" t="s">
+      <c r="D70" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="556"/>
+      <c r="E70" s="567"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>2892974.0700000003</v>
@@ -23008,22 +23035,22 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="557" t="s">
+      <c r="D71" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="557"/>
+      <c r="E71" s="568"/>
       <c r="F71" s="101">
         <v>-931631.77</v>
       </c>
-      <c r="I71" s="558" t="s">
+      <c r="I71" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="559"/>
-      <c r="K71" s="560">
+      <c r="J71" s="570"/>
+      <c r="K71" s="571">
         <f>F73+F74+F75</f>
         <v>4814667.01</v>
       </c>
-      <c r="L71" s="560"/>
+      <c r="L71" s="571"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -23068,11 +23095,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="561">
+      <c r="K73" s="572">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="560"/>
+      <c r="L73" s="571"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -23093,22 +23120,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="549" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="550"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="551" t="s">
+      <c r="I75" s="562" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="552"/>
-      <c r="K75" s="553">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
         <v>1683279.9699999997</v>
       </c>
-      <c r="L75" s="553"/>
+      <c r="L75" s="564"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -23253,6 +23280,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -23269,12 +23302,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25722,8 +25749,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25749,23 +25776,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -25775,21 +25802,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -25808,14 +25835,14 @@
       <c r="D4" s="24">
         <v>45135</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -25825,7 +25852,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -25977,7 +26004,7 @@
         <v>152870</v>
       </c>
       <c r="Q7" s="45">
-        <f t="shared" ref="Q6:Q39" si="1">P7-F7</f>
+        <f t="shared" ref="Q7:Q39" si="1">P7-F7</f>
         <v>0</v>
       </c>
       <c r="R7" s="46">
@@ -26258,30 +26285,38 @@
       <c r="B13" s="32">
         <v>45144</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="33">
+        <v>19252</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>897</v>
+      </c>
       <c r="E13" s="35">
         <v>45144</v>
       </c>
-      <c r="F13" s="36"/>
+      <c r="F13" s="36">
+        <v>104305</v>
+      </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38">
         <v>45144</v>
       </c>
-      <c r="I13" s="39"/>
+      <c r="I13" s="39">
+        <v>1265.5</v>
+      </c>
       <c r="J13" s="40"/>
       <c r="K13" s="343"/>
       <c r="L13" s="49"/>
       <c r="M13" s="42">
-        <v>0</v>
+        <v>43061.5</v>
       </c>
       <c r="N13" s="43">
-        <v>0</v>
+        <v>40726</v>
       </c>
       <c r="O13" s="192"/>
       <c r="P13" s="49">
         <f>N13+M13+L13+I13+C13</f>
-        <v>0</v>
+        <v>104305</v>
       </c>
       <c r="Q13" s="45">
         <f t="shared" si="1"/>
@@ -26302,30 +26337,39 @@
       <c r="B14" s="32">
         <v>45145</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="33">
+        <v>39840</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>898</v>
+      </c>
       <c r="E14" s="35">
         <v>45145</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="36">
+        <v>207595</v>
+      </c>
       <c r="G14" s="37"/>
       <c r="H14" s="38">
         <v>45145</v>
       </c>
-      <c r="I14" s="39"/>
+      <c r="I14" s="39">
+        <v>1816</v>
+      </c>
       <c r="J14" s="40"/>
       <c r="K14" s="65"/>
       <c r="L14" s="49"/>
       <c r="M14" s="42">
-        <v>0</v>
+        <f>87614+1430</f>
+        <v>89044</v>
       </c>
       <c r="N14" s="43">
-        <v>0</v>
+        <v>76895</v>
       </c>
       <c r="O14" s="193"/>
       <c r="P14" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>207595</v>
       </c>
       <c r="Q14" s="45">
         <f t="shared" si="1"/>
@@ -26346,29 +26390,38 @@
       <c r="B15" s="32">
         <v>45146</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="33">
+        <v>19759</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>899</v>
+      </c>
       <c r="E15" s="35">
         <v>45146</v>
       </c>
-      <c r="F15" s="36"/>
+      <c r="F15" s="36">
+        <v>173547</v>
+      </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38">
         <v>45146</v>
       </c>
-      <c r="I15" s="39"/>
+      <c r="I15" s="39">
+        <v>2143</v>
+      </c>
       <c r="J15" s="40"/>
       <c r="K15" s="65"/>
       <c r="L15" s="49"/>
       <c r="M15" s="42">
-        <v>0</v>
+        <f>79794+12191+3456</f>
+        <v>95441</v>
       </c>
       <c r="N15" s="43">
-        <v>0</v>
+        <v>56204</v>
       </c>
       <c r="P15" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>173547</v>
       </c>
       <c r="Q15" s="45">
         <f t="shared" si="1"/>
@@ -26389,29 +26442,38 @@
       <c r="B16" s="32">
         <v>45147</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="33">
+        <v>17177</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>900</v>
+      </c>
       <c r="E16" s="35">
         <v>45147</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="36">
+        <v>121787</v>
+      </c>
       <c r="G16" s="37"/>
       <c r="H16" s="38">
         <v>45147</v>
       </c>
-      <c r="I16" s="39"/>
+      <c r="I16" s="39">
+        <v>2919</v>
+      </c>
       <c r="J16" s="40"/>
       <c r="K16" s="342"/>
       <c r="L16" s="13"/>
       <c r="M16" s="42">
-        <v>0</v>
+        <f>46373+2307+5507</f>
+        <v>54187</v>
       </c>
       <c r="N16" s="43">
-        <v>0</v>
+        <v>47504</v>
       </c>
       <c r="P16" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>121787</v>
       </c>
       <c r="Q16" s="45">
         <f t="shared" si="1"/>
@@ -26434,30 +26496,39 @@
       <c r="B17" s="32">
         <v>45148</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="47"/>
+      <c r="C17" s="33">
+        <v>5345</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>901</v>
+      </c>
       <c r="E17" s="35">
         <v>45148</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="36">
+        <v>234342</v>
+      </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38">
         <v>45148</v>
       </c>
-      <c r="I17" s="39"/>
+      <c r="I17" s="39">
+        <v>2555</v>
+      </c>
       <c r="J17" s="40"/>
       <c r="K17" s="65"/>
       <c r="L17" s="55"/>
       <c r="M17" s="42">
-        <v>0</v>
+        <f>120207+12818+2165</f>
+        <v>135190</v>
       </c>
       <c r="N17" s="43">
-        <v>0</v>
+        <v>91252</v>
       </c>
       <c r="O17" s="499"/>
       <c r="P17" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>234342</v>
       </c>
       <c r="Q17" s="45">
         <f t="shared" si="1"/>
@@ -26478,29 +26549,37 @@
       <c r="B18" s="32">
         <v>45149</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="33">
+        <v>7541</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>902</v>
+      </c>
       <c r="E18" s="35">
         <v>45149</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="36">
+        <v>150157</v>
+      </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38">
         <v>45149</v>
       </c>
-      <c r="I18" s="39"/>
+      <c r="I18" s="39">
+        <v>1889</v>
+      </c>
       <c r="J18" s="40"/>
       <c r="K18" s="58"/>
       <c r="L18" s="49"/>
       <c r="M18" s="42">
-        <v>0</v>
+        <v>88736</v>
       </c>
       <c r="N18" s="43">
-        <v>0</v>
+        <v>51991</v>
       </c>
       <c r="P18" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150157</v>
       </c>
       <c r="Q18" s="45">
         <f t="shared" si="1"/>
@@ -26521,39 +26600,56 @@
       <c r="B19" s="32">
         <v>45150</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="33">
+        <v>18046</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>903</v>
+      </c>
       <c r="E19" s="35">
         <v>45150</v>
       </c>
-      <c r="F19" s="36"/>
+      <c r="F19" s="36">
+        <v>186919</v>
+      </c>
       <c r="G19" s="37"/>
       <c r="H19" s="38">
         <v>45150</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="344"/>
-      <c r="L19" s="59"/>
+      <c r="I19" s="39">
+        <v>5426</v>
+      </c>
+      <c r="J19" s="40">
+        <v>45150</v>
+      </c>
+      <c r="K19" s="344" t="s">
+        <v>904</v>
+      </c>
+      <c r="L19" s="59">
+        <v>33661.81</v>
+      </c>
       <c r="M19" s="42">
-        <v>0</v>
+        <f>58832+500+4094</f>
+        <v>63426</v>
       </c>
       <c r="N19" s="43">
-        <v>0</v>
+        <v>66272</v>
       </c>
       <c r="O19" s="499"/>
       <c r="P19" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="45">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>186831.81</v>
+      </c>
+      <c r="Q19" s="404">
+        <f t="shared" si="1"/>
+        <v>-87.190000000002328</v>
       </c>
       <c r="R19" s="46">
         <v>0</v>
       </c>
-      <c r="S19" s="233"/>
+      <c r="S19" s="233" t="s">
+        <v>97</v>
+      </c>
       <c r="T19" s="233"/>
       <c r="U19" s="233"/>
       <c r="V19" s="233"/>
@@ -27402,7 +27498,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="45">
-        <f t="shared" ref="Q6:Q47" si="2">P41-F41</f>
+        <f t="shared" ref="Q41:Q47" si="2">P41-F41</f>
         <v>0</v>
       </c>
       <c r="R41" s="46">
@@ -27491,9 +27587,15 @@
       <c r="G44" s="37"/>
       <c r="H44" s="38"/>
       <c r="I44" s="103"/>
-      <c r="J44" s="338"/>
-      <c r="K44" s="471"/>
-      <c r="L44" s="49"/>
+      <c r="J44" s="338">
+        <v>45150</v>
+      </c>
+      <c r="K44" s="471" t="s">
+        <v>905</v>
+      </c>
+      <c r="L44" s="49">
+        <v>18826.84</v>
+      </c>
       <c r="M44" s="42">
         <v>0</v>
       </c>
@@ -27639,21 +27741,21 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
-        <v>672792.5</v>
-      </c>
-      <c r="N49" s="554">
+        <v>1241878</v>
+      </c>
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
-        <v>497620</v>
+        <v>928464</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>1362716</v>
-      </c>
-      <c r="Q49" s="566">
+        <v>2541280.81</v>
+      </c>
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
-        <v>0</v>
+        <v>-87.190000000002328</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -27672,10 +27774,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>2184</v>
@@ -27730,11 +27832,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
-        <v>1170412.5</v>
-      </c>
-      <c r="N53" s="569"/>
+        <v>2170342</v>
+      </c>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -27973,7 +28075,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>118222.5</v>
+        <v>245182.5</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -27981,7 +28083,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>1360532</v>
+        <v>2539184</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -27989,7 +28091,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>20356</v>
+        <v>38369.5</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -27997,7 +28099,7 @@
       </c>
       <c r="L67" s="527">
         <f>SUM(L5:L65)-L26</f>
-        <v>102070.6</v>
+        <v>154559.25</v>
       </c>
       <c r="M67" s="150"/>
       <c r="N67" s="150"/>
@@ -28015,50 +28117,50 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="562" t="s">
+      <c r="H69" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="563"/>
+      <c r="I69" s="574"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="564">
+      <c r="K69" s="575">
         <f>I67+L67</f>
-        <v>122426.6</v>
-      </c>
-      <c r="L69" s="565"/>
+        <v>192928.75</v>
+      </c>
+      <c r="L69" s="576"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="556" t="s">
+      <c r="D70" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="556"/>
+      <c r="E70" s="567"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>1119882.8999999999</v>
+        <v>2101072.75</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="557" t="s">
+      <c r="D71" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="557"/>
+      <c r="E71" s="568"/>
       <c r="F71" s="101">
         <v>0</v>
       </c>
-      <c r="I71" s="558" t="s">
+      <c r="I71" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="559"/>
-      <c r="K71" s="560">
+      <c r="J71" s="570"/>
+      <c r="K71" s="571">
         <f>F73+F74+F75</f>
-        <v>4266343.5600000005</v>
-      </c>
-      <c r="L71" s="560"/>
+        <v>5247533.41</v>
+      </c>
+      <c r="L71" s="571"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -28096,18 +28198,18 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>1119882.8999999999</v>
+        <v>2101072.75</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="561">
+      <c r="K73" s="572">
         <f>-C4</f>
         <v>-2820551.31</v>
       </c>
-      <c r="L73" s="560"/>
+      <c r="L73" s="571"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -28128,22 +28230,22 @@
       <c r="C75" s="172">
         <v>45171</v>
       </c>
-      <c r="D75" s="549" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="550"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="173">
         <v>3146460.66</v>
       </c>
-      <c r="I75" s="551" t="s">
+      <c r="I75" s="562" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="552"/>
-      <c r="K75" s="553">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
-        <v>1445792.2500000005</v>
-      </c>
-      <c r="L75" s="553"/>
+        <v>2426982.1</v>
+      </c>
+      <c r="L75" s="564"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -28288,13 +28390,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -28310,6 +28405,13 @@
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
+    <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33263,23 +33365,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -33289,24 +33391,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="543" t="s">
+      <c r="R3" s="554" t="s">
         <v>3</v>
       </c>
     </row>
@@ -33321,14 +33423,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -33338,11 +33440,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="544"/>
+      <c r="R4" s="555"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -35318,11 +35420,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -35330,7 +35432,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -35363,10 +35465,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -35457,11 +35559,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -36020,26 +36122,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="562" t="s">
+      <c r="H77" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="563"/>
+      <c r="I77" s="574"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="564">
+      <c r="K77" s="575">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="565"/>
+      <c r="L77" s="576"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="556" t="s">
+      <c r="D78" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="556"/>
+      <c r="E78" s="567"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -36048,22 +36150,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="557" t="s">
+      <c r="D79" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="557"/>
+      <c r="E79" s="568"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="558" t="s">
+      <c r="I79" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="559"/>
-      <c r="K79" s="560">
+      <c r="J79" s="570"/>
+      <c r="K79" s="571">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="560"/>
+      <c r="L79" s="571"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -36104,11 +36206,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="561">
+      <c r="K81" s="572">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="560"/>
+      <c r="L81" s="571"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -36125,10 +36227,10 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="549" t="s">
+      <c r="D83" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="550"/>
+      <c r="E83" s="561"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
@@ -36287,6 +36389,12 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -36303,12 +36411,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -39020,23 +39122,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -39046,21 +39148,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="599" t="s">
@@ -39078,14 +39180,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -39095,7 +39197,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -41080,11 +41182,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -41092,7 +41194,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -41125,10 +41227,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -41219,11 +41321,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -41702,26 +41804,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="562" t="s">
+      <c r="H77" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="563"/>
+      <c r="I77" s="574"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="564">
+      <c r="K77" s="575">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="565"/>
+      <c r="L77" s="576"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="556" t="s">
+      <c r="D78" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="556"/>
+      <c r="E78" s="567"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -41730,22 +41832,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="557" t="s">
+      <c r="D79" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="557"/>
+      <c r="E79" s="568"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="558" t="s">
+      <c r="I79" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="559"/>
-      <c r="K79" s="560">
+      <c r="J79" s="570"/>
+      <c r="K79" s="571">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="560"/>
+      <c r="L79" s="571"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -41786,11 +41888,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="561">
+      <c r="K81" s="572">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="560"/>
+      <c r="L81" s="571"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -41807,22 +41909,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="549" t="s">
+      <c r="D83" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="550"/>
+      <c r="E83" s="561"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="551" t="s">
+      <c r="I83" s="562" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="552"/>
-      <c r="K83" s="553">
+      <c r="J83" s="563"/>
+      <c r="K83" s="564">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="553"/>
+      <c r="L83" s="564"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -41969,12 +42071,6 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -41991,6 +42087,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44564,23 +44666,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -44590,21 +44692,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="599" t="s">
@@ -44622,14 +44724,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -44639,7 +44741,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -46664,11 +46766,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -46676,7 +46778,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -46703,10 +46805,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -46780,11 +46882,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -47413,26 +47515,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="562" t="s">
+      <c r="H79" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="563"/>
+      <c r="I79" s="574"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="564">
+      <c r="K79" s="575">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="565"/>
+      <c r="L79" s="576"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="556" t="s">
+      <c r="D80" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="556"/>
+      <c r="E80" s="567"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -47441,22 +47543,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="557" t="s">
+      <c r="D81" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="557"/>
+      <c r="E81" s="568"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="558" t="s">
+      <c r="I81" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="559"/>
-      <c r="K81" s="560">
+      <c r="J81" s="570"/>
+      <c r="K81" s="571">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="560"/>
+      <c r="L81" s="571"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -47497,11 +47599,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="561">
+      <c r="K83" s="572">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="560"/>
+      <c r="L83" s="571"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -47518,22 +47620,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="549" t="s">
+      <c r="D85" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="550"/>
+      <c r="E85" s="561"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="551" t="s">
+      <c r="I85" s="562" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="552"/>
-      <c r="K85" s="553">
+      <c r="J85" s="563"/>
+      <c r="K85" s="564">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="553"/>
+      <c r="L85" s="564"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -47681,6 +47783,12 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47697,12 +47805,6 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -50357,23 +50459,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="572"/>
-      <c r="C1" s="574" t="s">
+      <c r="B1" s="547"/>
+      <c r="C1" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="575"/>
-      <c r="E1" s="575"/>
-      <c r="F1" s="575"/>
-      <c r="G1" s="575"/>
-      <c r="H1" s="575"/>
-      <c r="I1" s="575"/>
-      <c r="J1" s="575"/>
-      <c r="K1" s="575"/>
-      <c r="L1" s="575"/>
-      <c r="M1" s="575"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
+      <c r="K1" s="550"/>
+      <c r="L1" s="550"/>
+      <c r="M1" s="550"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="573"/>
+      <c r="B2" s="548"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -50383,21 +50485,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="576" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="577"/>
+      <c r="B3" s="551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="552"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="578" t="s">
+      <c r="H3" s="553" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="578"/>
+      <c r="I3" s="553"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="570" t="s">
+      <c r="P3" s="545" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -50418,14 +50520,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="556" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="546"/>
-      <c r="H4" s="547" t="s">
+      <c r="F4" s="557"/>
+      <c r="H4" s="558" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="559"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -50435,7 +50537,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="571"/>
+      <c r="P4" s="546"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -52442,11 +52544,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="554">
+      <c r="M49" s="565">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="554">
+      <c r="N49" s="565">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -52454,7 +52556,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="566">
+      <c r="Q49" s="577">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -52487,10 +52589,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="555"/>
-      <c r="N50" s="555"/>
+      <c r="M50" s="566"/>
+      <c r="N50" s="566"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="567"/>
+      <c r="Q50" s="578"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -52569,11 +52671,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="568">
+      <c r="M53" s="543">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="569"/>
+      <c r="N53" s="544"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -53052,26 +53154,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="562" t="s">
+      <c r="H77" s="573" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="563"/>
+      <c r="I77" s="574"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="564">
+      <c r="K77" s="575">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="565"/>
+      <c r="L77" s="576"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="556" t="s">
+      <c r="D78" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="556"/>
+      <c r="E78" s="567"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -53080,22 +53182,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="557" t="s">
+      <c r="D79" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="557"/>
+      <c r="E79" s="568"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="558" t="s">
+      <c r="I79" s="569" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="559"/>
-      <c r="K79" s="560">
+      <c r="J79" s="570"/>
+      <c r="K79" s="571">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="560"/>
+      <c r="L79" s="571"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -53136,11 +53238,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="561">
+      <c r="K81" s="572">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="560"/>
+      <c r="L81" s="571"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -53157,10 +53259,10 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="549" t="s">
+      <c r="D83" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="550"/>
+      <c r="E83" s="561"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
@@ -53320,12 +53422,6 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -53342,6 +53438,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 16 SEPT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/BALANCE  ZAVALETA   AGOSTO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/BALANCE  ZAVALETA   AGOSTO    2023.xlsx
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="921">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -3384,6 +3384,9 @@
   </si>
   <si>
     <t>ARABE-VERDURA-POLLO-QUESOS-SALCHICHA</t>
+  </si>
+  <si>
+    <t>pollo</t>
   </si>
 </sst>
 </file>
@@ -6091,39 +6094,6 @@
     <xf numFmtId="16" fontId="23" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6198,6 +6168,39 @@
     </xf>
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10076,23 +10079,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -10102,24 +10105,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="556" t="s">
+      <c r="R3" s="545" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10134,14 +10137,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -10151,11 +10154,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="557"/>
+      <c r="R4" s="546"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -11990,11 +11993,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -12002,7 +12005,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -12023,10 +12026,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -12081,11 +12084,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -12510,26 +12513,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="575" t="s">
+      <c r="H77" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="576"/>
+      <c r="I77" s="565"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="577">
+      <c r="K77" s="566">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="578"/>
+      <c r="L77" s="567"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="569" t="s">
+      <c r="D78" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="569"/>
+      <c r="E78" s="558"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -12538,22 +12541,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="570" t="s">
+      <c r="D79" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="570"/>
+      <c r="E79" s="559"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="571" t="s">
+      <c r="I79" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="572"/>
-      <c r="K79" s="573">
+      <c r="J79" s="561"/>
+      <c r="K79" s="562">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="573"/>
+      <c r="L79" s="562"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -12594,11 +12597,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="574">
+      <c r="K81" s="563">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="573"/>
+      <c r="L81" s="562"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -12615,22 +12618,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="562" t="s">
+      <c r="D83" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="563"/>
+      <c r="E83" s="552"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="564" t="s">
+      <c r="I83" s="553" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="565"/>
-      <c r="K83" s="566">
+      <c r="J83" s="554"/>
+      <c r="K83" s="555">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="566"/>
+      <c r="L83" s="555"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -12777,6 +12780,12 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -12793,12 +12802,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15197,23 +15200,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -15223,21 +15226,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -15258,14 +15261,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -15275,7 +15278,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -17335,11 +17338,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -17347,7 +17350,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -17380,10 +17383,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -17468,11 +17471,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -17801,26 +17804,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="575" t="s">
+      <c r="H69" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="576"/>
+      <c r="I69" s="565"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="577">
+      <c r="K69" s="566">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="578"/>
+      <c r="L69" s="567"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="569" t="s">
+      <c r="D70" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="569"/>
+      <c r="E70" s="558"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -17829,23 +17832,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="570" t="s">
+      <c r="D71" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="570"/>
+      <c r="E71" s="559"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="571" t="s">
+      <c r="I71" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="572"/>
-      <c r="K71" s="573">
+      <c r="J71" s="561"/>
+      <c r="K71" s="562">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="573"/>
+      <c r="L71" s="562"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -17887,11 +17890,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="574">
+      <c r="K73" s="563">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="573"/>
+      <c r="L73" s="562"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -17908,22 +17911,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="562" t="s">
+      <c r="D75" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="563"/>
+      <c r="E75" s="552"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="564" t="s">
+      <c r="I75" s="553" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="565"/>
-      <c r="K75" s="566">
+      <c r="J75" s="554"/>
+      <c r="K75" s="555">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="566"/>
+      <c r="L75" s="555"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -18071,12 +18074,6 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -18093,6 +18090,12 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -20492,23 +20495,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -20518,21 +20521,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -20551,14 +20554,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -20568,7 +20571,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -22659,11 +22662,11 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>2422108.7600000002</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1603736</v>
       </c>
@@ -22671,7 +22674,7 @@
         <f>SUM(P5:P40)</f>
         <v>4927758.76</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>-0.23999999999068677</v>
       </c>
@@ -22698,10 +22701,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>440369</v>
@@ -22768,11 +22771,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>4025844.7600000002</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -23055,26 +23058,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="575" t="s">
+      <c r="H69" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="576"/>
+      <c r="I69" s="565"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="577">
+      <c r="K69" s="566">
         <f>I67+L67</f>
         <v>594414.23</v>
       </c>
-      <c r="L69" s="578"/>
+      <c r="L69" s="567"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="569" t="s">
+      <c r="D70" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="569"/>
+      <c r="E70" s="558"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>2892974.0700000003</v>
@@ -23083,22 +23086,22 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="570" t="s">
+      <c r="D71" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="570"/>
+      <c r="E71" s="559"/>
       <c r="F71" s="101">
         <v>-931631.77</v>
       </c>
-      <c r="I71" s="571" t="s">
+      <c r="I71" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="572"/>
-      <c r="K71" s="573">
+      <c r="J71" s="561"/>
+      <c r="K71" s="562">
         <f>F73+F74+F75</f>
         <v>4814667.01</v>
       </c>
-      <c r="L71" s="573"/>
+      <c r="L71" s="562"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -23143,11 +23146,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="574">
+      <c r="K73" s="563">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="573"/>
+      <c r="L73" s="562"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -23168,22 +23171,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="562" t="s">
+      <c r="D75" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="563"/>
+      <c r="E75" s="552"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="564" t="s">
+      <c r="I75" s="553" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="565"/>
-      <c r="K75" s="566">
+      <c r="J75" s="554"/>
+      <c r="K75" s="555">
         <f>K71+K73</f>
         <v>1683279.9699999997</v>
       </c>
-      <c r="L75" s="566"/>
+      <c r="L75" s="555"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -23328,12 +23331,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -23350,6 +23347,12 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25797,8 +25800,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25824,23 +25827,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -25850,21 +25853,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -25883,14 +25886,14 @@
       <c r="D4" s="24">
         <v>45135</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -25900,7 +25903,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -27267,38 +27270,44 @@
       <c r="B31" s="32">
         <v>45162</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="79"/>
+      <c r="C31" s="33">
+        <v>2070</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>920</v>
+      </c>
       <c r="E31" s="35">
         <v>45162</v>
       </c>
-      <c r="F31" s="36" t="s">
-        <v>10</v>
+      <c r="F31" s="36">
+        <v>140850</v>
       </c>
       <c r="G31" s="37"/>
       <c r="H31" s="38">
         <v>45162</v>
       </c>
-      <c r="I31" s="39"/>
+      <c r="I31" s="39">
+        <v>1675</v>
+      </c>
       <c r="J31" s="338"/>
       <c r="K31" s="347"/>
       <c r="L31" s="68"/>
       <c r="M31" s="42">
-        <v>0</v>
+        <v>90791</v>
       </c>
       <c r="N31" s="43">
-        <v>0</v>
+        <v>46314</v>
       </c>
       <c r="P31" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="45" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R31" s="46">
-        <v>0</v>
+        <v>140850</v>
+      </c>
+      <c r="Q31" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="46" t="s">
+        <v>10</v>
       </c>
       <c r="S31" s="233"/>
     </row>
@@ -27907,21 +27916,21 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
-        <v>2166427.23</v>
-      </c>
-      <c r="N49" s="567">
+        <v>2257218.23</v>
+      </c>
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
-        <v>1515459</v>
+        <v>1561773</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>4324743.54</v>
-      </c>
-      <c r="Q49" s="579" t="e">
+        <v>4465593.54</v>
+      </c>
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
-        <v>#VALUE!</v>
+        <v>-130072.45999999999</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -27940,10 +27949,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>146522</v>
@@ -27998,11 +28007,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
-        <v>3681886.23</v>
-      </c>
-      <c r="N53" s="546"/>
+        <v>3818991.23</v>
+      </c>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -28241,7 +28250,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>455779</v>
+        <v>457849</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -28249,7 +28258,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>4308294</v>
+        <v>4449144</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -28257,7 +28266,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>73975.5</v>
+        <v>75650.5</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -28283,50 +28292,50 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="575" t="s">
+      <c r="H69" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="576"/>
+      <c r="I69" s="565"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="577">
+      <c r="K69" s="566">
         <f>I67+L67</f>
-        <v>258658.02</v>
-      </c>
-      <c r="L69" s="578"/>
+        <v>260333.02</v>
+      </c>
+      <c r="L69" s="567"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="569" t="s">
+      <c r="D70" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="569"/>
+      <c r="E70" s="558"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>3593856.98</v>
+        <v>3730961.98</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="570" t="s">
+      <c r="D71" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="570"/>
+      <c r="E71" s="559"/>
       <c r="F71" s="101">
         <v>0</v>
       </c>
-      <c r="I71" s="571" t="s">
+      <c r="I71" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="572"/>
-      <c r="K71" s="573">
+      <c r="J71" s="561"/>
+      <c r="K71" s="562">
         <f>F73+F74+F75</f>
-        <v>6740317.6400000006</v>
-      </c>
-      <c r="L71" s="573"/>
+        <v>6877422.6400000006</v>
+      </c>
+      <c r="L71" s="562"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -28360,18 +28369,18 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>3593856.98</v>
+        <v>3730961.98</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="574">
+      <c r="K73" s="563">
         <f>-C4</f>
         <v>-2820551.31</v>
       </c>
-      <c r="L73" s="573"/>
+      <c r="L73" s="562"/>
       <c r="O73" s="536"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -28389,22 +28398,22 @@
       <c r="C75" s="172">
         <v>45171</v>
       </c>
-      <c r="D75" s="562" t="s">
+      <c r="D75" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="563"/>
+      <c r="E75" s="552"/>
       <c r="F75" s="173">
         <v>3146460.66</v>
       </c>
-      <c r="I75" s="564" t="s">
+      <c r="I75" s="553" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="565"/>
-      <c r="K75" s="566">
+      <c r="J75" s="554"/>
+      <c r="K75" s="555">
         <f>K71+K73</f>
-        <v>3919766.3300000005</v>
-      </c>
-      <c r="L75" s="566"/>
+        <v>4056871.3300000005</v>
+      </c>
+      <c r="L75" s="555"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -28549,6 +28558,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -28565,12 +28580,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33524,23 +33533,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -33550,24 +33559,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="556" t="s">
+      <c r="R3" s="545" t="s">
         <v>3</v>
       </c>
     </row>
@@ -33582,14 +33591,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -33599,11 +33608,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="557"/>
+      <c r="R4" s="546"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -35579,11 +35588,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -35591,7 +35600,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -35624,10 +35633,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -35718,11 +35727,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -36281,26 +36290,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="575" t="s">
+      <c r="H77" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="576"/>
+      <c r="I77" s="565"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="577">
+      <c r="K77" s="566">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="578"/>
+      <c r="L77" s="567"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="569" t="s">
+      <c r="D78" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="569"/>
+      <c r="E78" s="558"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -36309,22 +36318,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="570" t="s">
+      <c r="D79" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="570"/>
+      <c r="E79" s="559"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="571" t="s">
+      <c r="I79" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="572"/>
-      <c r="K79" s="573">
+      <c r="J79" s="561"/>
+      <c r="K79" s="562">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="573"/>
+      <c r="L79" s="562"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -36365,11 +36374,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="574">
+      <c r="K81" s="563">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="573"/>
+      <c r="L81" s="562"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -36386,10 +36395,10 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="562" t="s">
+      <c r="D83" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="563"/>
+      <c r="E83" s="552"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
@@ -36548,12 +36557,6 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -36570,6 +36573,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -39281,23 +39290,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -39307,21 +39316,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="601" t="s">
@@ -39339,14 +39348,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -39356,7 +39365,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -41341,11 +41350,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -41353,7 +41362,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -41386,10 +41395,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -41480,11 +41489,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -41963,26 +41972,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="575" t="s">
+      <c r="H77" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="576"/>
+      <c r="I77" s="565"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="577">
+      <c r="K77" s="566">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="578"/>
+      <c r="L77" s="567"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="569" t="s">
+      <c r="D78" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="569"/>
+      <c r="E78" s="558"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -41991,22 +42000,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="570" t="s">
+      <c r="D79" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="570"/>
+      <c r="E79" s="559"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="571" t="s">
+      <c r="I79" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="572"/>
-      <c r="K79" s="573">
+      <c r="J79" s="561"/>
+      <c r="K79" s="562">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="573"/>
+      <c r="L79" s="562"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -42047,11 +42056,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="574">
+      <c r="K81" s="563">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="573"/>
+      <c r="L81" s="562"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -42068,22 +42077,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="562" t="s">
+      <c r="D83" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="563"/>
+      <c r="E83" s="552"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="564" t="s">
+      <c r="I83" s="553" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="565"/>
-      <c r="K83" s="566">
+      <c r="J83" s="554"/>
+      <c r="K83" s="555">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="566"/>
+      <c r="L83" s="555"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -42230,6 +42239,12 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -42246,12 +42261,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44825,23 +44834,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -44851,21 +44860,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="601" t="s">
@@ -44883,14 +44892,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -44900,7 +44909,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -46925,11 +46934,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -46937,7 +46946,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -46964,10 +46973,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -47041,11 +47050,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -47674,26 +47683,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="575" t="s">
+      <c r="H79" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="576"/>
+      <c r="I79" s="565"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="577">
+      <c r="K79" s="566">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="578"/>
+      <c r="L79" s="567"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="569" t="s">
+      <c r="D80" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="569"/>
+      <c r="E80" s="558"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -47702,22 +47711,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="570" t="s">
+      <c r="D81" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="570"/>
+      <c r="E81" s="559"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="571" t="s">
+      <c r="I81" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="572"/>
-      <c r="K81" s="573">
+      <c r="J81" s="561"/>
+      <c r="K81" s="562">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="573"/>
+      <c r="L81" s="562"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -47758,11 +47767,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="574">
+      <c r="K83" s="563">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="573"/>
+      <c r="L83" s="562"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -47779,22 +47788,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="562" t="s">
+      <c r="D85" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="563"/>
+      <c r="E85" s="552"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="564" t="s">
+      <c r="I85" s="553" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="565"/>
-      <c r="K85" s="566">
+      <c r="J85" s="554"/>
+      <c r="K85" s="555">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="566"/>
+      <c r="L85" s="555"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -47942,12 +47951,6 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47964,6 +47967,12 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -50618,23 +50627,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="549"/>
-      <c r="C1" s="551" t="s">
+      <c r="B1" s="574"/>
+      <c r="C1" s="576" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
-      <c r="L1" s="552"/>
-      <c r="M1" s="552"/>
+      <c r="D1" s="577"/>
+      <c r="E1" s="577"/>
+      <c r="F1" s="577"/>
+      <c r="G1" s="577"/>
+      <c r="H1" s="577"/>
+      <c r="I1" s="577"/>
+      <c r="J1" s="577"/>
+      <c r="K1" s="577"/>
+      <c r="L1" s="577"/>
+      <c r="M1" s="577"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="550"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -50644,21 +50653,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="554"/>
+      <c r="B3" s="578" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="579"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="580" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="580"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="547" t="s">
+      <c r="P3" s="572" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -50679,14 +50688,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="558" t="s">
+      <c r="E4" s="547" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="559"/>
-      <c r="H4" s="560" t="s">
+      <c r="F4" s="548"/>
+      <c r="H4" s="549" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="561"/>
+      <c r="I4" s="550"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -50696,7 +50705,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="548"/>
+      <c r="P4" s="573"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -52703,11 +52712,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="567">
+      <c r="M49" s="556">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="567">
+      <c r="N49" s="556">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -52715,7 +52724,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="579">
+      <c r="Q49" s="568">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -52748,10 +52757,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="568"/>
-      <c r="N50" s="568"/>
+      <c r="M50" s="557"/>
+      <c r="N50" s="557"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="580"/>
+      <c r="Q50" s="569"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -52830,11 +52839,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="545">
+      <c r="M53" s="570">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="546"/>
+      <c r="N53" s="571"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -53313,26 +53322,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="575" t="s">
+      <c r="H77" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="576"/>
+      <c r="I77" s="565"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="577">
+      <c r="K77" s="566">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="578"/>
+      <c r="L77" s="567"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="569" t="s">
+      <c r="D78" s="558" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="569"/>
+      <c r="E78" s="558"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -53341,22 +53350,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="570" t="s">
+      <c r="D79" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="570"/>
+      <c r="E79" s="559"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="571" t="s">
+      <c r="I79" s="560" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="572"/>
-      <c r="K79" s="573">
+      <c r="J79" s="561"/>
+      <c r="K79" s="562">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="573"/>
+      <c r="L79" s="562"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -53397,11 +53406,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="574">
+      <c r="K81" s="563">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="573"/>
+      <c r="L81" s="562"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -53418,10 +53427,10 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="562" t="s">
+      <c r="D83" s="551" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="563"/>
+      <c r="E83" s="552"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
@@ -53581,6 +53590,12 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -53597,12 +53612,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>